<commit_message>
Made a very minor change
</commit_message>
<xml_diff>
--- a/Git commands.xlsx
+++ b/Git commands.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F274162-47B3-469C-91F4-264CFBD4C2E8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE595874-0239-43D1-9949-8624C7CB5EE9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="47">
   <si>
     <t>To check the version of git installed</t>
   </si>
@@ -75,9 +75,6 @@
     <t>git config --list</t>
   </si>
   <si>
-    <t>git clone https://github.com/kishoreramanna/datasciencecoursera.git</t>
-  </si>
-  <si>
     <t>ls</t>
   </si>
   <si>
@@ -90,16 +87,7 @@
     <t>git status</t>
   </si>
   <si>
-    <t>git username configuration</t>
-  </si>
-  <si>
-    <t>git email configuration</t>
-  </si>
-  <si>
     <t>check the git configuration</t>
-  </si>
-  <si>
-    <t>Clone a remote repo to your local i.e. create a copy of repository from github to your local computer</t>
   </si>
   <si>
     <t>Just do this once</t>
@@ -167,17 +155,57 @@
 Once the push command returns, then we can check the results in github</t>
   </si>
   <si>
-    <t>rm ./datasciencecoursera -rf</t>
+    <t>rm ./basicGitcommands -rf</t>
+  </si>
+  <si>
+    <t>Sets the name you want attached to your commit transactions</t>
+  </si>
+  <si>
+    <t>Sets the email you want attached to your commit transactions</t>
+  </si>
+  <si>
+    <t>git config --global color.ui auto</t>
+  </si>
+  <si>
+    <t>Enables helpful colorization of command line output</t>
+  </si>
+  <si>
+    <t>git init [project-name]</t>
+  </si>
+  <si>
+    <t>Creates a new local repository with the specified name</t>
+  </si>
+  <si>
+    <t>git clone https://github.com/kishoreramanna/basicGitcommands.git</t>
+  </si>
+  <si>
+    <t>Downloads a remote repo project and its entire version history to your local</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -191,7 +219,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -214,35 +242,35 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -264,13 +292,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>106680</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>589657</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>1335251</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -278,7 +306,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{19E654D2-2893-499D-8F7A-CF952680E07F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{48A47BEE-44DF-43B0-A475-DFBBCF320E3B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -294,7 +322,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8648700" y="2301240"/>
+          <a:off x="8526780" y="5562600"/>
           <a:ext cx="7142857" cy="1228571"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -308,21 +336,21 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>160020</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>15240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>378229</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>49313</xdr:rowOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>834173</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{48C4DB46-B424-483D-8AEF-D4B3BA01034A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D7BF56F-8BB3-4768-933A-1746EB788637}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -338,7 +366,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8656320" y="4221480"/>
+          <a:off x="8534400" y="7482840"/>
           <a:ext cx="6923809" cy="1733333"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -352,13 +380,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>152400</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>83820</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>389657</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>1264772</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -366,7 +394,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25D263D3-FAEC-40B7-8AE0-673744C2CAEA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{23AA680D-711A-4505-98D0-4B562D1AEC7C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -382,7 +410,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8648700" y="6172200"/>
+          <a:off x="8526780" y="9433560"/>
           <a:ext cx="6942857" cy="1180952"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -396,13 +424,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>236220</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>128593</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
       <xdr:colOff>560433</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>2039613</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -410,7 +438,7 @@
         <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0C45F802-94AE-458F-ADD1-7807487CF358}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE0EBABA-C8F6-4893-94DF-9CF2710D4890}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -426,7 +454,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8732520" y="2323153"/>
+          <a:off x="8610600" y="3359473"/>
           <a:ext cx="4591413" cy="1911020"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -440,13 +468,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>83820</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>144780</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>530601</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>24</xdr:row>
       <xdr:rowOff>1085710</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -454,7 +482,7 @@
         <xdr:cNvPr id="6" name="Picture 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E6810F38-157F-4A5F-A4EC-82F5A59AA1A5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1CDFB7AD-645A-463A-BE1D-7A88C645D53C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -470,7 +498,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8580120" y="10020300"/>
+          <a:off x="8458200" y="11056620"/>
           <a:ext cx="7152381" cy="1123810"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -745,28 +773,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E24"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{432A978F-3057-41D8-B203-1CE62C2D22FC}">
+  <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="60.77734375" customWidth="1"/>
+    <col min="2" max="2" width="59" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="56.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="5" t="s">
         <v>3</v>
       </c>
     </row>
@@ -830,13 +858,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" t="s">
-        <v>25</v>
+        <v>38</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
@@ -844,184 +869,218 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
       <c r="D8" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>15</v>
+      <c r="B9" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>23</v>
+        <v>40</v>
+      </c>
+      <c r="D9" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>16</v>
+      <c r="B10" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D10" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="E10" s="4" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
-      <c r="B11" s="1" t="s">
-        <v>17</v>
+      <c r="B11" s="2" t="s">
+        <v>15</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="38.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>11</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C12" s="1" t="s">
+      <c r="B12" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" s="8"/>
+    </row>
+    <row r="13" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
         <v>12</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="175.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="B13" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>27</v>
+        <v>16</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
-        <v>13</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>28</v>
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="175.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
-        <v>14</v>
-      </c>
-      <c r="B16" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
         <v>17</v>
       </c>
-      <c r="C16" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="1">
-        <v>15</v>
-      </c>
-      <c r="B17" s="1" t="s">
+      <c r="B18" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="133.80000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="1">
-        <v>16</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="1" t="s">
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C24" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="144" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="123" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="1">
-        <v>18</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A21" s="1">
-        <v>19</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="A22" s="1">
-        <v>20</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C22" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="144" x14ac:dyDescent="0.3">
-      <c r="A23" s="2">
-        <v>21</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C23" s="5" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="C24" s="6"/>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C27" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>